<commit_message>
Touch on G Drive
Same files, but file attributes changed by new version of Google Drive.
</commit_message>
<xml_diff>
--- a/data/ConversionFactors.xlsx
+++ b/data/ConversionFactors.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Google Drive/Zia Lab/Codebase/qdef/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5002E0CC-C7E9-6B4B-94F5-453DE96004F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681908F7-9402-464C-9E08-3B6DA94BEF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="18000" activeTab="1" xr2:uid="{AAAE55A6-0C68-0541-BB78-4F67D14A1699}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="18000" xr2:uid="{AAAE55A6-0C68-0541-BB78-4F67D14A1699}"/>
   </bookViews>
   <sheets>
-    <sheet name="lengths" sheetId="1" r:id="rId1"/>
-    <sheet name="energy" sheetId="2" r:id="rId2"/>
-    <sheet name="energy_equivs" sheetId="3" r:id="rId3"/>
-    <sheet name="mass" sheetId="4" r:id="rId4"/>
+    <sheet name="time" sheetId="5" r:id="rId1"/>
+    <sheet name="lengths" sheetId="1" r:id="rId2"/>
+    <sheet name="energy" sheetId="2" r:id="rId3"/>
+    <sheet name="energy_equivs" sheetId="3" r:id="rId4"/>
+    <sheet name="mass" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="106">
   <si>
     <t>m</t>
   </si>
@@ -280,6 +281,81 @@
   </si>
   <si>
     <t>watthour</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>μs</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>ps</t>
+  </si>
+  <si>
+    <t>fs</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>kHz</t>
+  </si>
+  <si>
+    <t>GHz</t>
+  </si>
+  <si>
+    <t>THz</t>
+  </si>
+  <si>
+    <t>Hertz</t>
+  </si>
+  <si>
+    <t>kilohertz</t>
+  </si>
+  <si>
+    <t>metahertz</t>
+  </si>
+  <si>
+    <t>gigahertz</t>
+  </si>
+  <si>
+    <t>terarhertz</t>
+  </si>
+  <si>
+    <t>femtpsecond</t>
+  </si>
+  <si>
+    <t>picosecond</t>
+  </si>
+  <si>
+    <t>nanosecond</t>
+  </si>
+  <si>
+    <t>microsecond</t>
+  </si>
+  <si>
+    <t>milisecond</t>
   </si>
 </sst>
 </file>
@@ -631,6 +707,232 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0802372-976C-CF42-B6A0-750DE3A6A820}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1000000000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1000000000000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1000000000000000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8273698B-D5E8-B044-874B-D6BB6F470FB3}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -884,11 +1186,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE195A5-F53F-094E-B172-A5DC4E7C6C13}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1243,12 +1545,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50993A46-4EFA-994D-B632-C1210228ABFC}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1297,7 +1599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F9A786-42D0-934C-A010-A2195A2DB393}">
   <dimension ref="A1:E6"/>
   <sheetViews>

</xml_diff>

<commit_message>
SansGT and assorted fixes here and there
+ Fixed unit conversion spreadsheet.
+ matrixdooogies.py includes routine to block diagonalize a sparse matrix.
+ qdef.py now includes a function to generate a symbolic expression for a Hamiltonian that includes both crystal field and Coulomb repulsion terms.
+SansGT.ipynb include the development code for hamiltonian_CF_CR and example of use.
+ A method was added to Qet that allows applying sp.simplify to the values of a Qet.
</commit_message>
<xml_diff>
--- a/data/ConversionFactors.xlsx
+++ b/data/ConversionFactors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Google Drive/Zia Lab/Codebase/qdef/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Zia Lab/Codebase/qdef/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681908F7-9402-464C-9E08-3B6DA94BEF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BECF4D3-0622-6445-9547-78D6080372C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="18000" xr2:uid="{AAAE55A6-0C68-0541-BB78-4F67D14A1699}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="21600" windowHeight="18000" activeTab="3" xr2:uid="{AAAE55A6-0C68-0541-BB78-4F67D14A1699}"/>
   </bookViews>
   <sheets>
     <sheet name="time" sheetId="5" r:id="rId1"/>
@@ -710,7 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0802372-976C-CF42-B6A0-750DE3A6A820}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -937,7 +937,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1154,7 +1154,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="1">
-        <v>0.01</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -1549,7 +1549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50993A46-4EFA-994D-B632-C1210228ABFC}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>